<commit_message>
Atualiza dados de uso das plataformas Matific e Speak para 2025
</commit_message>
<xml_diff>
--- a/MATIFIC  2025  por semana inicio na semana 1  (1) (1).xlsx
+++ b/MATIFIC  2025  por semana inicio na semana 1  (1) (1).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\regina.pieruchi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davi.silva\AppData\Local\Packages\5319275A.WhatsAppDesktop_cv1g1gvanyjgm\LocalState\sessions\AC76DCD02D74194452A54312DB1979B0DFABA41A\transfers\2025-51\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E208DF-E141-4056-B5E7-C31E891E5E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234CBFE9-C4F1-4A50-8656-C01CA5ED33E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A913360B-ABA4-474C-A115-2935233947B5}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A913360B-ABA4-474C-A115-2935233947B5}"/>
   </bookViews>
   <sheets>
     <sheet name="MATIFIC" sheetId="1" r:id="rId1"/>
@@ -1341,6 +1341,57 @@
     <xf numFmtId="2" fontId="10" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="8" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1376,57 +1427,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1759,8 +1759,7 @@
   <dimension ref="A1:BA38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B5" sqref="B5"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1794,80 +1793,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="110" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="129" t="s">
+      <c r="C1" s="118" t="s">
         <v>107</v>
       </c>
-      <c r="D1" s="130"/>
-      <c r="E1" s="130"/>
-      <c r="F1" s="130"/>
-      <c r="G1" s="130"/>
-      <c r="H1" s="130"/>
-      <c r="I1" s="130"/>
-      <c r="J1" s="130"/>
-      <c r="K1" s="130"/>
-      <c r="L1" s="130"/>
-      <c r="M1" s="131"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="119"/>
+      <c r="J1" s="119"/>
+      <c r="K1" s="119"/>
+      <c r="L1" s="119"/>
+      <c r="M1" s="120"/>
       <c r="N1" s="16" t="s">
         <v>40</v>
       </c>
       <c r="O1" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="P1" s="129" t="s">
+      <c r="P1" s="118" t="s">
         <v>105</v>
       </c>
-      <c r="Q1" s="130"/>
-      <c r="R1" s="130"/>
-      <c r="S1" s="130"/>
-      <c r="T1" s="130"/>
-      <c r="U1" s="130"/>
-      <c r="V1" s="131"/>
+      <c r="Q1" s="119"/>
+      <c r="R1" s="119"/>
+      <c r="S1" s="119"/>
+      <c r="T1" s="119"/>
+      <c r="U1" s="119"/>
+      <c r="V1" s="120"/>
       <c r="W1" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="X1" s="126" t="s">
+      <c r="X1" s="115" t="s">
         <v>96</v>
       </c>
-      <c r="Y1" s="127"/>
-      <c r="Z1" s="127"/>
-      <c r="AA1" s="127"/>
-      <c r="AB1" s="127"/>
-      <c r="AC1" s="127"/>
-      <c r="AD1" s="127"/>
-      <c r="AE1" s="127"/>
-      <c r="AF1" s="127"/>
-      <c r="AG1" s="127"/>
-      <c r="AH1" s="127"/>
-      <c r="AI1" s="128"/>
-      <c r="AJ1" s="116" t="s">
+      <c r="Y1" s="116"/>
+      <c r="Z1" s="116"/>
+      <c r="AA1" s="116"/>
+      <c r="AB1" s="116"/>
+      <c r="AC1" s="116"/>
+      <c r="AD1" s="116"/>
+      <c r="AE1" s="116"/>
+      <c r="AF1" s="116"/>
+      <c r="AG1" s="116"/>
+      <c r="AH1" s="116"/>
+      <c r="AI1" s="117"/>
+      <c r="AJ1" s="105" t="s">
         <v>86</v>
       </c>
-      <c r="AK1" s="117"/>
-      <c r="AL1" s="117"/>
-      <c r="AM1" s="117"/>
-      <c r="AN1" s="117"/>
-      <c r="AO1" s="117"/>
-      <c r="AP1" s="117"/>
-      <c r="AQ1" s="117"/>
-      <c r="AR1" s="117"/>
-      <c r="AS1" s="117"/>
-      <c r="AT1" s="117"/>
-      <c r="AU1" s="117"/>
-      <c r="AV1" s="117"/>
-      <c r="AW1" s="117"/>
-      <c r="AX1" s="117"/>
-      <c r="AY1" s="117"/>
-      <c r="AZ1" s="117"/>
-      <c r="BA1" s="118"/>
+      <c r="AK1" s="106"/>
+      <c r="AL1" s="106"/>
+      <c r="AM1" s="106"/>
+      <c r="AN1" s="106"/>
+      <c r="AO1" s="106"/>
+      <c r="AP1" s="106"/>
+      <c r="AQ1" s="106"/>
+      <c r="AR1" s="106"/>
+      <c r="AS1" s="106"/>
+      <c r="AT1" s="106"/>
+      <c r="AU1" s="106"/>
+      <c r="AV1" s="106"/>
+      <c r="AW1" s="106"/>
+      <c r="AX1" s="106"/>
+      <c r="AY1" s="106"/>
+      <c r="AZ1" s="106"/>
+      <c r="BA1" s="107"/>
     </row>
     <row r="2" spans="1:53" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="122"/>
+      <c r="A2" s="111"/>
       <c r="B2" s="18" t="s">
         <v>45</v>
       </c>
@@ -1978,11 +1977,11 @@
       <c r="AM2" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="AN2" s="119" t="s">
+      <c r="AN2" s="108" t="s">
         <v>52</v>
       </c>
-      <c r="AO2" s="120"/>
-      <c r="AP2" s="124" t="s">
+      <c r="AO2" s="109"/>
+      <c r="AP2" s="113" t="s">
         <v>64</v>
       </c>
       <c r="AQ2" s="28" t="s">
@@ -2020,7 +2019,7 @@
       </c>
     </row>
     <row r="3" spans="1:53" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="123"/>
+      <c r="A3" s="112"/>
       <c r="B3" s="30" t="s">
         <v>117</v>
       </c>
@@ -2131,7 +2130,7 @@
       <c r="AO3" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="AP3" s="125"/>
+      <c r="AP3" s="114"/>
       <c r="AQ3" s="36" t="s">
         <v>33</v>
       </c>
@@ -3559,7 +3558,7 @@
         <v>16</v>
       </c>
       <c r="B13" s="38"/>
-      <c r="C13" s="132">
+      <c r="C13" s="104">
         <f t="shared" si="0"/>
         <v>0.3831</v>
       </c>
@@ -3865,7 +3864,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="38"/>
-      <c r="C15" s="132">
+      <c r="C15" s="104">
         <f t="shared" si="0"/>
         <v>0.97689999999999999</v>
       </c>
@@ -5375,84 +5374,84 @@
     </row>
     <row r="30" spans="1:53" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="1:53" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="AE31" s="104" t="s">
+      <c r="AE31" s="121" t="s">
         <v>57</v>
       </c>
-      <c r="AF31" s="114"/>
-      <c r="AG31" s="114"/>
-      <c r="AH31" s="114"/>
-      <c r="AI31" s="114"/>
-      <c r="AJ31" s="114"/>
-      <c r="AK31" s="114"/>
-      <c r="AL31" s="115"/>
-      <c r="AQ31" s="104" t="s">
+      <c r="AF31" s="131"/>
+      <c r="AG31" s="131"/>
+      <c r="AH31" s="131"/>
+      <c r="AI31" s="131"/>
+      <c r="AJ31" s="131"/>
+      <c r="AK31" s="131"/>
+      <c r="AL31" s="132"/>
+      <c r="AQ31" s="121" t="s">
         <v>57</v>
       </c>
-      <c r="AR31" s="105"/>
-      <c r="AS31" s="105"/>
-      <c r="AT31" s="106"/>
+      <c r="AR31" s="122"/>
+      <c r="AS31" s="122"/>
+      <c r="AT31" s="123"/>
     </row>
     <row r="32" spans="1:53" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="AE32" s="4"/>
       <c r="AF32" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AG32" s="113" t="s">
+      <c r="AG32" s="130" t="s">
         <v>58</v>
       </c>
-      <c r="AH32" s="113"/>
-      <c r="AI32" s="113"/>
-      <c r="AJ32" s="113"/>
-      <c r="AK32" s="113"/>
-      <c r="AL32" s="113"/>
+      <c r="AH32" s="130"/>
+      <c r="AI32" s="130"/>
+      <c r="AJ32" s="130"/>
+      <c r="AK32" s="130"/>
+      <c r="AL32" s="130"/>
       <c r="AQ32" s="2"/>
-      <c r="AR32" s="107" t="s">
+      <c r="AR32" s="124" t="s">
         <v>61</v>
       </c>
-      <c r="AS32" s="108"/>
-      <c r="AT32" s="109"/>
+      <c r="AS32" s="125"/>
+      <c r="AT32" s="126"/>
     </row>
     <row r="33" spans="30:46" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="AE33" s="6"/>
       <c r="AF33" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="AG33" s="113" t="s">
+      <c r="AG33" s="130" t="s">
         <v>59</v>
       </c>
-      <c r="AH33" s="113"/>
-      <c r="AI33" s="113"/>
-      <c r="AJ33" s="113"/>
-      <c r="AK33" s="113"/>
-      <c r="AL33" s="113"/>
+      <c r="AH33" s="130"/>
+      <c r="AI33" s="130"/>
+      <c r="AJ33" s="130"/>
+      <c r="AK33" s="130"/>
+      <c r="AL33" s="130"/>
       <c r="AP33" s="8"/>
       <c r="AQ33" s="1"/>
-      <c r="AR33" s="110" t="s">
+      <c r="AR33" s="127" t="s">
         <v>62</v>
       </c>
-      <c r="AS33" s="111"/>
-      <c r="AT33" s="112"/>
+      <c r="AS33" s="128"/>
+      <c r="AT33" s="129"/>
     </row>
     <row r="34" spans="30:46" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="AE34" s="7"/>
       <c r="AF34" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="AG34" s="113" t="s">
+      <c r="AG34" s="130" t="s">
         <v>60</v>
       </c>
-      <c r="AH34" s="113"/>
-      <c r="AI34" s="113"/>
-      <c r="AJ34" s="113"/>
-      <c r="AK34" s="113"/>
-      <c r="AL34" s="113"/>
+      <c r="AH34" s="130"/>
+      <c r="AI34" s="130"/>
+      <c r="AJ34" s="130"/>
+      <c r="AK34" s="130"/>
+      <c r="AL34" s="130"/>
       <c r="AP34" s="8"/>
       <c r="AQ34" s="3"/>
-      <c r="AR34" s="107" t="s">
+      <c r="AR34" s="124" t="s">
         <v>63</v>
       </c>
-      <c r="AS34" s="108"/>
-      <c r="AT34" s="109"/>
+      <c r="AS34" s="125"/>
+      <c r="AT34" s="126"/>
     </row>
     <row r="35" spans="30:46" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AE35" s="11"/>
@@ -5509,13 +5508,6 @@
     <sortCondition descending="1" ref="AQ4:AQ29"/>
   </sortState>
   <mergeCells count="15">
-    <mergeCell ref="AJ1:BA1"/>
-    <mergeCell ref="AN2:AO2"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="AP2:AP3"/>
-    <mergeCell ref="X1:AI1"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="P1:V1"/>
     <mergeCell ref="AQ31:AT31"/>
     <mergeCell ref="AR32:AT32"/>
     <mergeCell ref="AR33:AT33"/>
@@ -5524,6 +5516,13 @@
     <mergeCell ref="AG33:AL33"/>
     <mergeCell ref="AG34:AL34"/>
     <mergeCell ref="AE31:AL31"/>
+    <mergeCell ref="AJ1:BA1"/>
+    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="AP2:AP3"/>
+    <mergeCell ref="X1:AI1"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="P1:V1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>